<commit_message>
Atualiza datasets e ajustes das ligas
</commit_message>
<xml_diff>
--- a/libertadores/datasets_liberta/classificacao_por_grupo_fase_1.xlsx
+++ b/libertadores/datasets_liberta/classificacao_por_grupo_fase_1.xlsx
@@ -104,10 +104,10 @@
     <t>A Lenda Super Vasco F.c</t>
   </si>
   <si>
-    <t>BORGES ITAQUI F.C.</t>
-  </si>
-  <si>
     <t>FBC Colorado</t>
+  </si>
+  <si>
+    <t>Grêmio imortal 36</t>
   </si>
   <si>
     <t>Mau Humor F.C.</t>

</xml_diff>

<commit_message>
Atualiza parciais e avisos na Libertadores
</commit_message>
<xml_diff>
--- a/libertadores/datasets_liberta/classificacao_por_grupo_fase_1.xlsx
+++ b/libertadores/datasets_liberta/classificacao_por_grupo_fase_1.xlsx
@@ -56,51 +56,54 @@
     <t>Grupo A</t>
   </si>
   <si>
+    <t>Tatols Beants F.C</t>
+  </si>
+  <si>
+    <t>JV5 Tricolor Gaúcho</t>
+  </si>
+  <si>
     <t>JUV. KP</t>
   </si>
   <si>
-    <t>JV5 Tricolor Gaúcho</t>
-  </si>
-  <si>
     <t>SERGRILLO</t>
   </si>
   <si>
-    <t>Tatols Beants F.C</t>
-  </si>
-  <si>
     <t>Grupo B</t>
   </si>
   <si>
+    <t>S.E.R. GRILLO</t>
+  </si>
+  <si>
     <t>Dom Camillo68</t>
   </si>
   <si>
+    <t>Máquina Laranjja</t>
+  </si>
+  <si>
     <t>LISI GREMISTA</t>
   </si>
   <si>
-    <t>Máquina Laranjja</t>
-  </si>
-  <si>
-    <t>S.E.R. GRILLO</t>
-  </si>
-  <si>
     <t>Grupo C</t>
   </si>
   <si>
+    <t>dasdoresfc</t>
+  </si>
+  <si>
     <t>Bandoleros FCS</t>
   </si>
   <si>
     <t>cartola scheuer17</t>
   </si>
   <si>
-    <t>dasdoresfc</t>
-  </si>
-  <si>
     <t>seralex</t>
   </si>
   <si>
     <t>Grupo D</t>
   </si>
   <si>
+    <t>Mau Humor F.C.</t>
+  </si>
+  <si>
     <t>A Lenda Super Vasco F.c</t>
   </si>
   <si>
@@ -110,67 +113,64 @@
     <t>Grêmio imortal 36</t>
   </si>
   <si>
-    <t>Mau Humor F.C.</t>
-  </si>
-  <si>
     <t>Grupo E</t>
   </si>
   <si>
+    <t>Paulo Virgili FC</t>
+  </si>
+  <si>
+    <t>KillerColorado</t>
+  </si>
+  <si>
     <t>Fedato Futebol Clube</t>
   </si>
   <si>
     <t>FÚRIA LEON</t>
   </si>
   <si>
-    <t>KillerColorado</t>
-  </si>
-  <si>
-    <t>Paulo Virgili FC</t>
-  </si>
-  <si>
     <t>Grupo F</t>
   </si>
   <si>
+    <t>lsauer fc</t>
+  </si>
+  <si>
+    <t>Rolo Compressor ZN</t>
+  </si>
+  <si>
+    <t>DM Studio</t>
+  </si>
+  <si>
     <t>AZURRA82</t>
   </si>
   <si>
-    <t>DM Studio</t>
-  </si>
-  <si>
-    <t>Rolo Compressor ZN</t>
-  </si>
-  <si>
-    <t>lsauer fc</t>
-  </si>
-  <si>
     <t>Grupo G</t>
   </si>
   <si>
+    <t>TORRESMO COM PINGA PRO26.1</t>
+  </si>
+  <si>
+    <t>Tabajara de Inhaua PB1</t>
+  </si>
+  <si>
     <t>A Lenda Super Vascão f.c</t>
   </si>
   <si>
     <t>Grêmio imortal 37</t>
   </si>
   <si>
-    <t>TORRESMO COM PINGA PRO26.1</t>
-  </si>
-  <si>
-    <t>Tabajara de Inhaua PB1</t>
-  </si>
-  <si>
     <t>Grupo H</t>
   </si>
   <si>
+    <t>Texas Club 2026</t>
+  </si>
+  <si>
     <t>Gremiomaniasm</t>
   </si>
   <si>
+    <t>TEAM LOPES 99</t>
+  </si>
+  <si>
     <t>Super Vasco f.c</t>
-  </si>
-  <si>
-    <t>TEAM LOPES 99</t>
-  </si>
-  <si>
-    <t>Texas Club 2026</t>
   </si>
 </sst>
 </file>
@@ -574,10 +574,10 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -586,13 +586,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>64.95999999999999</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>41.6</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>23.35999999999999</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -606,10 +606,10 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -618,13 +618,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>39.66</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>38.5</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1.159999999999997</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -647,16 +647,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>41.6</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>64.95999999999999</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-23.35999999999999</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -679,16 +679,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>38.5</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>39.66</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>-1.159999999999997</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -747,10 +747,10 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -759,13 +759,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>59.76</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>45.86</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>13.9</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -779,10 +779,10 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -791,13 +791,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>58.4</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>39.66</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>18.74</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -820,16 +820,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>45.86</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>59.76</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-13.9</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -852,16 +852,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>39.66</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>58.4</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>-18.74</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -920,10 +920,10 @@
         <v>21</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -932,13 +932,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>71.36</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>34.36</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -952,10 +952,10 @@
         <v>22</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -964,13 +964,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>69.56</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>53.06</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>16.5</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -993,16 +993,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>53.06</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>69.56</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-16.5</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1025,16 +1025,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>34.36</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>71.36</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>-37</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -1093,10 +1093,10 @@
         <v>26</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1105,13 +1105,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>69.76000000000001</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>45.46</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>24.3</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1125,10 +1125,10 @@
         <v>27</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1137,13 +1137,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>59.56</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>30.6</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>28.96</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1166,16 +1166,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>45.46</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>69.76000000000001</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-24.3</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1198,16 +1198,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>30.6</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>59.56</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>-28.96</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -1266,10 +1266,10 @@
         <v>31</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1278,13 +1278,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>73.66</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>50.6</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>23.06</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1298,10 +1298,10 @@
         <v>32</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1310,13 +1310,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>57.25</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>49.16</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>8.090000000000003</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1339,16 +1339,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>50.6</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>73.66</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-23.06</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1371,16 +1371,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>49.16</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>57.25</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>-8.090000000000003</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -1439,10 +1439,10 @@
         <v>36</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1451,13 +1451,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>54.36</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>30.06</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>24.3</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1471,10 +1471,10 @@
         <v>37</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1483,13 +1483,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>51.05</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>47.2</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>3.849999999999994</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1512,16 +1512,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>47.2</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>51.05</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-3.849999999999994</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1544,16 +1544,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>30.06</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>54.36</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>-24.3</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -1612,10 +1612,10 @@
         <v>41</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1624,13 +1624,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>69.26000000000001</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>43.1</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>26.16</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1644,10 +1644,10 @@
         <v>42</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1656,13 +1656,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>57.76</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>45.3</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>12.46</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1685,16 +1685,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>45.3</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>57.76</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-12.46</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1717,16 +1717,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>43.1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>69.26000000000001</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>-26.16</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -1785,10 +1785,10 @@
         <v>46</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1797,13 +1797,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>59.86</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>50.76</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>9.100000000000001</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1817,10 +1817,10 @@
         <v>47</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1829,13 +1829,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>56.65</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>34.76</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>21.89</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1858,16 +1858,16 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>50.76</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>59.86</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-9.100000000000001</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1890,16 +1890,16 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>34.76</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>56.65</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>-21.89</v>
       </c>
       <c r="J5">
         <v>4</v>

</xml_diff>

<commit_message>
Automate notebook runs and refresh generated datasets
</commit_message>
<xml_diff>
--- a/libertadores/datasets_liberta/classificacao_por_grupo_fase_1.xlsx
+++ b/libertadores/datasets_liberta/classificacao_por_grupo_fase_1.xlsx
@@ -59,15 +59,15 @@
     <t>Tatols Beants F.C</t>
   </si>
   <si>
+    <t>SERGRILLO</t>
+  </si>
+  <si>
+    <t>JUV. KP</t>
+  </si>
+  <si>
     <t>JV5 Tricolor Gaúcho</t>
   </si>
   <si>
-    <t>JUV. KP</t>
-  </si>
-  <si>
-    <t>SERGRILLO</t>
-  </si>
-  <si>
     <t>Grupo B</t>
   </si>
   <si>
@@ -86,12 +86,12 @@
     <t>Grupo C</t>
   </si>
   <si>
+    <t>Bandoleros FCS</t>
+  </si>
+  <si>
     <t>dasdoresfc</t>
   </si>
   <si>
-    <t>Bandoleros FCS</t>
-  </si>
-  <si>
     <t>cartola scheuer17</t>
   </si>
   <si>
@@ -107,10 +107,10 @@
     <t>A Lenda Super Vasco F.c</t>
   </si>
   <si>
+    <t>Grêmio imortal 36</t>
+  </si>
+  <si>
     <t>FBC Colorado</t>
-  </si>
-  <si>
-    <t>Grêmio imortal 36</t>
   </si>
   <si>
     <t>Grupo E</t>
@@ -586,13 +586,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>64.95999999999999</v>
+        <v>66.86</v>
       </c>
       <c r="H2">
-        <v>41.6</v>
+        <v>46.79</v>
       </c>
       <c r="I2">
-        <v>23.35999999999999</v>
+        <v>20.07</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -618,13 +618,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>39.66</v>
+        <v>48.5</v>
       </c>
       <c r="H3">
-        <v>38.5</v>
+        <v>43.56</v>
       </c>
       <c r="I3">
-        <v>1.159999999999997</v>
+        <v>4.939999999999998</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -650,13 +650,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>41.6</v>
+        <v>46.79</v>
       </c>
       <c r="H4">
-        <v>64.95999999999999</v>
+        <v>66.86</v>
       </c>
       <c r="I4">
-        <v>-23.35999999999999</v>
+        <v>-20.07</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -682,13 +682,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>38.5</v>
+        <v>43.56</v>
       </c>
       <c r="H5">
-        <v>39.66</v>
+        <v>48.5</v>
       </c>
       <c r="I5">
-        <v>-1.159999999999997</v>
+        <v>-4.939999999999998</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -759,13 +759,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>59.76</v>
+        <v>65.06</v>
       </c>
       <c r="H2">
-        <v>45.86</v>
+        <v>47.16</v>
       </c>
       <c r="I2">
-        <v>13.9</v>
+        <v>17.90000000000001</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -791,13 +791,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>58.4</v>
+        <v>59.69</v>
       </c>
       <c r="H3">
-        <v>39.66</v>
+        <v>43.56</v>
       </c>
       <c r="I3">
-        <v>18.74</v>
+        <v>16.13</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -823,13 +823,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>45.86</v>
+        <v>47.16</v>
       </c>
       <c r="H4">
-        <v>59.76</v>
+        <v>65.06</v>
       </c>
       <c r="I4">
-        <v>-13.9</v>
+        <v>-17.90000000000001</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -855,13 +855,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>39.66</v>
+        <v>43.56</v>
       </c>
       <c r="H5">
-        <v>58.4</v>
+        <v>59.69</v>
       </c>
       <c r="I5">
-        <v>-18.74</v>
+        <v>-16.13</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -932,13 +932,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>71.36</v>
+        <v>71.45999999999999</v>
       </c>
       <c r="H2">
-        <v>34.36</v>
+        <v>57.26</v>
       </c>
       <c r="I2">
-        <v>37</v>
+        <v>14.2</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -964,13 +964,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>69.56</v>
+        <v>71.36</v>
       </c>
       <c r="H3">
-        <v>53.06</v>
+        <v>34.36</v>
       </c>
       <c r="I3">
-        <v>16.5</v>
+        <v>37</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -996,13 +996,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>53.06</v>
+        <v>57.26</v>
       </c>
       <c r="H4">
-        <v>69.56</v>
+        <v>71.45999999999999</v>
       </c>
       <c r="I4">
-        <v>-16.5</v>
+        <v>-14.2</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1105,13 +1105,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>69.76000000000001</v>
+        <v>71.36</v>
       </c>
       <c r="H2">
-        <v>45.46</v>
+        <v>49.36</v>
       </c>
       <c r="I2">
-        <v>24.3</v>
+        <v>22</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1137,13 +1137,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>59.56</v>
+        <v>63.76</v>
       </c>
       <c r="H3">
-        <v>30.6</v>
+        <v>50.69</v>
       </c>
       <c r="I3">
-        <v>28.96</v>
+        <v>13.07</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1169,13 +1169,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>45.46</v>
+        <v>50.69</v>
       </c>
       <c r="H4">
-        <v>69.76000000000001</v>
+        <v>63.76</v>
       </c>
       <c r="I4">
-        <v>-24.3</v>
+        <v>-13.07</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1201,13 +1201,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>30.6</v>
+        <v>49.36</v>
       </c>
       <c r="H5">
-        <v>59.56</v>
+        <v>71.36</v>
       </c>
       <c r="I5">
-        <v>-28.96</v>
+        <v>-22</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -1278,13 +1278,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>73.66</v>
+        <v>81.76000000000001</v>
       </c>
       <c r="H2">
-        <v>50.6</v>
+        <v>56.09</v>
       </c>
       <c r="I2">
-        <v>23.06</v>
+        <v>25.67</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1310,13 +1310,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>57.25</v>
+        <v>59.65</v>
       </c>
       <c r="H3">
-        <v>49.16</v>
+        <v>50.76</v>
       </c>
       <c r="I3">
-        <v>8.090000000000003</v>
+        <v>8.890000000000001</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1342,13 +1342,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>50.6</v>
+        <v>56.09</v>
       </c>
       <c r="H4">
-        <v>73.66</v>
+        <v>81.76000000000001</v>
       </c>
       <c r="I4">
-        <v>-23.06</v>
+        <v>-25.67</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1374,13 +1374,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>49.16</v>
+        <v>50.76</v>
       </c>
       <c r="H5">
-        <v>57.25</v>
+        <v>59.65</v>
       </c>
       <c r="I5">
-        <v>-8.090000000000003</v>
+        <v>-8.890000000000001</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -1451,10 +1451,10 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>54.36</v>
+        <v>58.26</v>
       </c>
       <c r="H2">
-        <v>30.06</v>
+        <v>33.96</v>
       </c>
       <c r="I2">
         <v>24.3</v>
@@ -1483,13 +1483,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>51.05</v>
+        <v>54.95</v>
       </c>
       <c r="H3">
-        <v>47.2</v>
+        <v>52.39</v>
       </c>
       <c r="I3">
-        <v>3.849999999999994</v>
+        <v>2.560000000000002</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1515,13 +1515,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>47.2</v>
+        <v>52.39</v>
       </c>
       <c r="H4">
-        <v>51.05</v>
+        <v>54.95</v>
       </c>
       <c r="I4">
-        <v>-3.849999999999994</v>
+        <v>-2.560000000000002</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1547,10 +1547,10 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>30.06</v>
+        <v>33.96</v>
       </c>
       <c r="H5">
-        <v>54.36</v>
+        <v>58.26</v>
       </c>
       <c r="I5">
         <v>-24.3</v>
@@ -1624,13 +1624,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>69.26000000000001</v>
+        <v>71.16</v>
       </c>
       <c r="H2">
-        <v>43.1</v>
+        <v>48.29</v>
       </c>
       <c r="I2">
-        <v>26.16</v>
+        <v>22.87</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1656,13 +1656,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>57.76</v>
+        <v>59.36</v>
       </c>
       <c r="H3">
-        <v>45.3</v>
+        <v>48.89</v>
       </c>
       <c r="I3">
-        <v>12.46</v>
+        <v>10.47</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1688,13 +1688,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>45.3</v>
+        <v>48.89</v>
       </c>
       <c r="H4">
-        <v>57.76</v>
+        <v>59.36</v>
       </c>
       <c r="I4">
-        <v>-12.46</v>
+        <v>-10.47</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1720,13 +1720,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>43.1</v>
+        <v>48.29</v>
       </c>
       <c r="H5">
-        <v>69.26000000000001</v>
+        <v>71.16</v>
       </c>
       <c r="I5">
-        <v>-26.16</v>
+        <v>-22.87</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -1797,10 +1797,10 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>59.86</v>
+        <v>63.76</v>
       </c>
       <c r="H2">
-        <v>50.76</v>
+        <v>54.66</v>
       </c>
       <c r="I2">
         <v>9.100000000000001</v>
@@ -1832,10 +1832,10 @@
         <v>56.65</v>
       </c>
       <c r="H3">
-        <v>34.76</v>
+        <v>38.66</v>
       </c>
       <c r="I3">
-        <v>21.89</v>
+        <v>17.99</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1861,10 +1861,10 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>50.76</v>
+        <v>54.66</v>
       </c>
       <c r="H4">
-        <v>59.86</v>
+        <v>63.76</v>
       </c>
       <c r="I4">
         <v>-9.100000000000001</v>
@@ -1893,13 +1893,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>34.76</v>
+        <v>38.66</v>
       </c>
       <c r="H5">
         <v>56.65</v>
       </c>
       <c r="I5">
-        <v>-21.89</v>
+        <v>-17.99</v>
       </c>
       <c r="J5">
         <v>4</v>

</xml_diff>

<commit_message>
Atualiza pontuacoes e resultados das competicoes
</commit_message>
<xml_diff>
--- a/libertadores/datasets_liberta/classificacao_por_grupo_fase_1.xlsx
+++ b/libertadores/datasets_liberta/classificacao_por_grupo_fase_1.xlsx
@@ -134,12 +134,12 @@
     <t>lsauer fc</t>
   </si>
   <si>
+    <t>DM Studio</t>
+  </si>
+  <si>
     <t>Rolo Compressor ZN</t>
   </si>
   <si>
-    <t>DM Studio</t>
-  </si>
-  <si>
     <t>AZURRA82</t>
   </si>
   <si>
@@ -152,10 +152,10 @@
     <t>Tabajara de Inhaua PB1</t>
   </si>
   <si>
+    <t>Grêmio imortal 37</t>
+  </si>
+  <si>
     <t>A Lenda Super Vascão f.c</t>
-  </si>
-  <si>
-    <t>Grêmio imortal 37</t>
   </si>
   <si>
     <t>Grupo H</t>
@@ -589,10 +589,10 @@
         <v>66.86</v>
       </c>
       <c r="H2">
-        <v>46.79</v>
+        <v>54.6</v>
       </c>
       <c r="I2">
-        <v>20.07</v>
+        <v>12.26</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -618,13 +618,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>48.5</v>
+        <v>49</v>
       </c>
       <c r="H3">
-        <v>43.56</v>
+        <v>47.86</v>
       </c>
       <c r="I3">
-        <v>4.939999999999998</v>
+        <v>1.140000000000001</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -650,13 +650,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>46.79</v>
+        <v>54.6</v>
       </c>
       <c r="H4">
         <v>66.86</v>
       </c>
       <c r="I4">
-        <v>-20.07</v>
+        <v>-12.26</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -682,13 +682,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>43.56</v>
+        <v>47.86</v>
       </c>
       <c r="H5">
-        <v>48.5</v>
+        <v>49</v>
       </c>
       <c r="I5">
-        <v>-4.939999999999998</v>
+        <v>-1.140000000000001</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -759,13 +759,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>65.06</v>
+        <v>84.86</v>
       </c>
       <c r="H2">
-        <v>47.16</v>
+        <v>49.76</v>
       </c>
       <c r="I2">
-        <v>17.90000000000001</v>
+        <v>35.1</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -791,13 +791,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>59.69</v>
+        <v>72.7</v>
       </c>
       <c r="H3">
-        <v>43.56</v>
+        <v>47.86</v>
       </c>
       <c r="I3">
-        <v>16.13</v>
+        <v>24.84</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -823,13 +823,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>47.16</v>
+        <v>49.76</v>
       </c>
       <c r="H4">
-        <v>65.06</v>
+        <v>84.86</v>
       </c>
       <c r="I4">
-        <v>-17.90000000000001</v>
+        <v>-35.1</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -855,13 +855,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>43.56</v>
+        <v>47.86</v>
       </c>
       <c r="H5">
-        <v>59.69</v>
+        <v>72.7</v>
       </c>
       <c r="I5">
-        <v>-16.13</v>
+        <v>-24.84</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -932,13 +932,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>71.45999999999999</v>
+        <v>74.06</v>
       </c>
       <c r="H2">
-        <v>57.26</v>
+        <v>61.56</v>
       </c>
       <c r="I2">
-        <v>14.2</v>
+        <v>12.5</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -964,13 +964,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>71.36</v>
+        <v>72.86</v>
       </c>
       <c r="H3">
-        <v>34.36</v>
+        <v>60.16</v>
       </c>
       <c r="I3">
-        <v>37</v>
+        <v>12.7</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -996,13 +996,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>57.26</v>
+        <v>61.56</v>
       </c>
       <c r="H4">
-        <v>71.45999999999999</v>
+        <v>74.06</v>
       </c>
       <c r="I4">
-        <v>-14.2</v>
+        <v>-12.5</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1028,13 +1028,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>34.36</v>
+        <v>60.16</v>
       </c>
       <c r="H5">
-        <v>71.36</v>
+        <v>72.86</v>
       </c>
       <c r="I5">
-        <v>-37</v>
+        <v>-12.7</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -1105,13 +1105,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>71.36</v>
+        <v>73.95999999999999</v>
       </c>
       <c r="H2">
-        <v>49.36</v>
+        <v>53.66</v>
       </c>
       <c r="I2">
-        <v>22</v>
+        <v>20.3</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1137,13 +1137,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>63.76</v>
+        <v>68.06</v>
       </c>
       <c r="H3">
-        <v>50.69</v>
+        <v>64.7</v>
       </c>
       <c r="I3">
-        <v>13.07</v>
+        <v>3.359999999999999</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1169,13 +1169,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>50.69</v>
+        <v>64.7</v>
       </c>
       <c r="H4">
-        <v>63.76</v>
+        <v>68.06</v>
       </c>
       <c r="I4">
-        <v>-13.07</v>
+        <v>-3.359999999999999</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1201,13 +1201,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>49.36</v>
+        <v>53.66</v>
       </c>
       <c r="H5">
-        <v>71.36</v>
+        <v>73.95999999999999</v>
       </c>
       <c r="I5">
-        <v>-22</v>
+        <v>-20.3</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -1278,13 +1278,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>81.76000000000001</v>
+        <v>84.26000000000001</v>
       </c>
       <c r="H2">
-        <v>56.09</v>
+        <v>63.9</v>
       </c>
       <c r="I2">
-        <v>25.67</v>
+        <v>20.36000000000001</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1310,13 +1310,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>59.65</v>
+        <v>72.45</v>
       </c>
       <c r="H3">
-        <v>50.76</v>
+        <v>54.16</v>
       </c>
       <c r="I3">
-        <v>8.890000000000001</v>
+        <v>18.29000000000001</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1342,13 +1342,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>56.09</v>
+        <v>63.9</v>
       </c>
       <c r="H4">
-        <v>81.76000000000001</v>
+        <v>84.26000000000001</v>
       </c>
       <c r="I4">
-        <v>-25.67</v>
+        <v>-20.36000000000001</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1374,13 +1374,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>50.76</v>
+        <v>54.16</v>
       </c>
       <c r="H5">
-        <v>59.65</v>
+        <v>72.45</v>
       </c>
       <c r="I5">
-        <v>-8.890000000000001</v>
+        <v>-18.29000000000001</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -1451,10 +1451,10 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>58.26</v>
+        <v>62.56</v>
       </c>
       <c r="H2">
-        <v>33.96</v>
+        <v>38.26</v>
       </c>
       <c r="I2">
         <v>24.3</v>
@@ -1483,13 +1483,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>54.95</v>
+        <v>60.2</v>
       </c>
       <c r="H3">
-        <v>52.39</v>
+        <v>59.25</v>
       </c>
       <c r="I3">
-        <v>2.560000000000002</v>
+        <v>0.9500000000000028</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1515,13 +1515,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>52.39</v>
+        <v>59.25</v>
       </c>
       <c r="H4">
-        <v>54.95</v>
+        <v>60.2</v>
       </c>
       <c r="I4">
-        <v>-2.560000000000002</v>
+        <v>-0.9500000000000028</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1547,10 +1547,10 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>33.96</v>
+        <v>38.26</v>
       </c>
       <c r="H5">
-        <v>58.26</v>
+        <v>62.56</v>
       </c>
       <c r="I5">
         <v>-24.3</v>
@@ -1624,13 +1624,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>71.16</v>
+        <v>73.76000000000001</v>
       </c>
       <c r="H2">
-        <v>48.29</v>
+        <v>57.6</v>
       </c>
       <c r="I2">
-        <v>22.87</v>
+        <v>16.16</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1656,13 +1656,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>59.36</v>
+        <v>61.96</v>
       </c>
       <c r="H3">
-        <v>48.89</v>
+        <v>54.1</v>
       </c>
       <c r="I3">
-        <v>10.47</v>
+        <v>7.859999999999999</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1688,13 +1688,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>48.89</v>
+        <v>57.6</v>
       </c>
       <c r="H4">
-        <v>59.36</v>
+        <v>73.76000000000001</v>
       </c>
       <c r="I4">
-        <v>-10.47</v>
+        <v>-16.16</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1720,13 +1720,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>48.29</v>
+        <v>54.1</v>
       </c>
       <c r="H5">
-        <v>71.16</v>
+        <v>61.96</v>
       </c>
       <c r="I5">
-        <v>-22.87</v>
+        <v>-7.859999999999999</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -1797,10 +1797,10 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>63.76</v>
+        <v>68.06</v>
       </c>
       <c r="H2">
-        <v>54.66</v>
+        <v>58.96</v>
       </c>
       <c r="I2">
         <v>9.100000000000001</v>
@@ -1829,13 +1829,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>56.65</v>
+        <v>57.45</v>
       </c>
       <c r="H3">
-        <v>38.66</v>
+        <v>42.96</v>
       </c>
       <c r="I3">
-        <v>17.99</v>
+        <v>14.49</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1861,10 +1861,10 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>54.66</v>
+        <v>58.96</v>
       </c>
       <c r="H4">
-        <v>63.76</v>
+        <v>68.06</v>
       </c>
       <c r="I4">
         <v>-9.100000000000001</v>
@@ -1893,13 +1893,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>38.66</v>
+        <v>42.96</v>
       </c>
       <c r="H5">
-        <v>56.65</v>
+        <v>57.45</v>
       </c>
       <c r="I5">
-        <v>-17.99</v>
+        <v>-14.49</v>
       </c>
       <c r="J5">
         <v>4</v>

</xml_diff>